<commit_message>
Added Datadriven test to Maddies
</commit_message>
<xml_diff>
--- a/MaddiesFramework/src/main/resources/configfile/testData.xlsx
+++ b/MaddiesFramework/src/main/resources/configfile/testData.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsingh5/git/latestPageObjectModelFramework/src/main/resources/configfile/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92AE3D8-8947-3F41-B8FF-1CFD477E437F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" activeTab="2" xr2:uid="{1E70CCEB-B519-2340-A0D6-827872CDD493}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6075" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="TestScripts" sheetId="2" r:id="rId2"/>
     <sheet name="LoginData" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Maddieslogindata" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:G9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Test Steps</t>
   </si>
@@ -94,12 +89,21 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>thimmaraju.g@winwire.com</t>
+  </si>
+  <si>
+    <t>winwiretestinghyd@gmail.com</t>
+  </si>
+  <si>
+    <t>cjsrsss@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -487,20 +491,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C113A96-F430-7948-86CC-28CFE8B182AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -514,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,7 +532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -542,7 +546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -556,7 +560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -576,16 +580,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B10E5B6-FCE8-474C-91C8-85328057A2E3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -593,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -601,7 +605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -609,7 +613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -624,20 +628,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06AD0CFE-F178-DB43-95FD-EA2A075B2340}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -651,7 +655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>18</v>
@@ -663,7 +667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>18</v>
@@ -675,7 +679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
@@ -688,9 +692,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{9CD3D93C-2FBA-BD4B-9477-D75209FABEE7}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{512EF6B6-3484-D04D-B889-69BE7B7B99C8}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{48AF9F90-9F5B-B04A-8876-7EEB3986E76D}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -698,13 +702,76 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8263DDFC-8FBD-EB47-B279-14F4A882BF1A}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123456</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1">
+        <v>456789</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1">
+        <v>123456</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
no changes ..removed name
</commit_message>
<xml_diff>
--- a/MaddiesFramework/src/main/resources/configfile/testData.xlsx
+++ b/MaddiesFramework/src/main/resources/configfile/testData.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WinWire\git\repository\MaddiesFramework\src\main\resources\configfile\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6075" activeTab="3"/>
+    <workbookView activeTab="1" windowHeight="3510" windowWidth="14835" xWindow="0" yWindow="2580"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="TestScripts" sheetId="2" r:id="rId2"/>
-    <sheet name="LoginData" sheetId="3" r:id="rId3"/>
-    <sheet name="Maddieslogindata" sheetId="4" r:id="rId4"/>
+    <sheet name="Login" r:id="rId1" sheetId="1"/>
+    <sheet name="TestScripts" r:id="rId2" sheetId="2"/>
+    <sheet name="LoginData" r:id="rId3" sheetId="3"/>
+    <sheet name="Maddieslogindata" r:id="rId4" sheetId="4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:K9"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
   <si>
     <t>Test Steps</t>
   </si>
@@ -62,50 +58,54 @@
     <t>Add to Cart</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>TestNameStart</t>
+  </si>
+  <si>
+    <t>LoginTestDataStart</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>runMode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>thimmaraju.g@winwire.com</t>
+  </si>
+  <si>
+    <t>winwiretestinghyd@gmail.com</t>
+  </si>
+  <si>
+    <t>cjsrsss@gmail.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>1529830551216@gmail.com</t>
   </si>
   <si>
     <t>FAIL</t>
   </si>
   <si>
-    <t>TestNameStart</t>
-  </si>
-  <si>
-    <t>LoginTestDataStart</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>runMode</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>thimmaraju.g@winwire.com</t>
-  </si>
-  <si>
-    <t>winwiretestinghyd@gmail.com</t>
-  </si>
-  <si>
-    <t>cjsrsss@gmail.com</t>
-  </si>
-  <si>
-    <t>password</t>
+    <t>fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -169,31 +169,31 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -210,10 +210,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -248,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -300,7 +300,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -411,21 +411,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -442,7 +442,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -494,29 +494,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -528,7 +528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -542,7 +542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -556,7 +556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -570,7 +570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -585,21 +585,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -607,182 +607,177 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="44.625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6">
-        <v>123456</v>
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6">
-        <v>456789</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6">
-        <v>123456</v>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="9" width="9.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>